<commit_message>
update order.xlsx input check
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -32,9 +32,6 @@
     <t>南京市江宁区正方中路888号南京中兴力维公司</t>
   </si>
   <si>
-    <t>新订</t>
-  </si>
-  <si>
     <t>南京市雨花台区紫荆花路68号</t>
   </si>
   <si>
@@ -95,9 +92,217 @@
     <t>即将离职发送到其他地址</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
+    <t xml:space="preserve">公司员工的名字，只在公司内部用于联系， 必填项目 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注。 （1）如果订过，这次的订购电话和之前的订购电话不同 ，请这里备注原来的订购电话号码，否则系统按号码查不到之前的订购情况，会按新订发版本，可能会重复版本。（2）复活用户或者零售转团购用户请打4008205099问清楚您所订购的到期“月号”并备注一下。（3） 如果清楚版本机制需要指定版本的，可以在这里备注订购版本，一般不建议这样。（4）注意如果有9月后的生日不满年龄提前上了幼儿园小班\中班\大班的，在备注中说明了，将按上学顺序发版本。 （5）如果不是联系人或者家长本人转账，也请备注转账人名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后请发邮件提交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购类型 ，不同类型区别在于发的订购礼物不同。巧虎公司根据电话号码和小朋友信息管理订购。新用户请选新订。续订是指到期后接着订购。复活是指中断后恢复订购。对复活和续订要填对原来订购的手机号便于接着之前订购情况发后继版本，巧虎公司会按手机号查询到历史订单确认最终订购类型。将提交给巧虎公司。请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>续订</t>
+  </si>
+  <si>
+    <t>订购周期，将提交给巧虎公司。新用户建议选1年（不可退订）。请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小朋友性别 ， 将提交给巧虎公司；请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购产品的家长性别，将提交给巧虎公司；请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号码 ，用于在巧虎公司订单系统查询之前的订单，确认本次订购方式，快递联系收货和用于对应售后服务，将提交给巧虎公司；复活或者续订用户如果这次要更换新的电话号码订购，请最后一项备注之前订购的电话号码。团购限制，一个手机号限订一份，除非同一个家庭的多个孩子可一个手机号码订多份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收货地址，将提交给巧虎公司；必填项目，一般限制为公司地址。
+特殊情况可选其他地址;请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如上面项选了需要发到其他地址，请填写详细的其他收货地址(包括省市）, 如提供将提交给巧虎公司。非必填项目。注意默认是家长收，电话也是上面的电话。不用新填收件人名字和电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>小朋友生日。格式为年月日，如20080808，出生年月关系到发的产品的版本内容的对应，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>请勿填错</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>；售后联系客服也需要提供这个生日。按上学顺序发版本；一般学龄前是宝宝版N月龄，托班发幼幼版，小班发快乐版，中班发成长版，大班发学习版，小学后是彩虹版和星空版。注意如果提前上幼儿园小班的，请在备注中说明，也可发快乐版。 提前上中班大班也请说明。已经是小学2年级拿星空版的订到下一个8月截止，不满1年请邮件联系我。注意最小是7月龄，最大是1年级。将提交给巧虎公司</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>联系邮箱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">。公司员工可填工号，如10088888，我将使用此工号在内部邮件系统中发邮件联系公司员工，确认付款和确认信息。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>注意</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>如果是需要直接联系其他的外网邮箱，不是联系公司员工确认付款和确认信息，请填外网邮箱。必填项目</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>感谢您的填写，注意1-11项是</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>必填</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">的。最后请确认上面填写的信息，特别是订购电话和小朋友生日，送货地址等重要信息无误后，使用常用邮箱发送到 qiaohu2013@qq.com  
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>一周内</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>您上面填的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>第3项的联系邮箱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>将收到确认收到团购信息和通知付款金额账号邮件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">。付款确认将统一在团购结束前发送。如果没收到上述邮件，请确认订购信息邮件是否发送成功，或联系邮箱 qiaohu2013@qq.com。
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color rgb="FF4B4B4B"/>
         <rFont val="宋体"/>
         <family val="3"/>
@@ -107,7 +312,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF4B4B4B"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -116,7 +321,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF4B4B4B"/>
         <rFont val="宋体"/>
         <family val="3"/>
@@ -124,176 +329,6 @@
       </rPr>
       <t>号</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">公司员工的名字，只在公司内部用于联系， 必填项目 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号码 ，用于在巧虎公司订单系统查询之前的订单，确认本次订购方式，快递联系收货和用于对应售后服务，将提交给巧虎公司；复活或者续订用户如果这次要更换新的电话号码订购，请最后一项备注之前订购的电话号码。团购限制，一个手机号限订一份，除非同一个家庭的多个孩子可一个手机号码订多份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>如上面项选了需要发到其他地址，请填写详细的其他收货地址(包括省市）, 如提供将提交给巧虎公司。非必填项目。注意默认是家长收，电话也是上面的电话。不用新填收件人名字和电话</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注。 （1）如果订过，这次的订购电话和之前的订购电话不同 ，请这里备注原来的订购电话号码，否则系统按号码查不到之前的订购情况，会按新订发版本，可能会重复版本。（2）复活用户或者零售转团购用户请打4008205099问清楚您所订购的到期“月号”并备注一下。（3） 如果清楚版本机制需要指定版本的，可以在这里备注订购版本，一般不建议这样。（4）注意如果有9月后的生日不满年龄提前上了幼儿园小班\中班\大班的，在备注中说明了，将按上学顺序发版本。 （5）如果不是联系人或者家长本人转账，也请备注转账人名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最后请发邮件提交</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>小朋友生日。格式为年月日，如20080808，出生年月关系到发的产品的版本内容的对应，</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>请勿填错</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>；售后联系客服也需要提供这个生日。按上学顺序发版本；一般学龄前是宝宝版N月龄，托班发幼幼版，小班发快乐版，中班发成长版，大班发学习版，小学后是彩虹版和星空版。注意如果提前上幼儿园小班的，请在备注中说明，也可发快乐版。 提前上中班大班也请说明。已经是小学2年级拿星空版的订到下一个8月截止，不满1年请邮件联系我。注意最小是7月龄，最大是1年级。将提交给巧虎公司</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>感谢您的填写，注意1-11项是</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>必填</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>的。最后请确认上面填写的信息，特别是订购电话和小朋友生日，送货地址等重要信息无误后，使用常用邮箱发送到 qiaohu2013@qq.com  
-   一周内您上面填的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>第3项的联系邮箱</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">将收到确认收到团购信息。后继会发通知付款金额账号邮件。付款确认将统一在团购结束前发送。如果没收到上述邮件，请确认订购信息邮件是否发送成功，或联系邮箱 qiaohu2013@qq.com。
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>联系邮箱</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">。公司员工可填工号，如10088888，我将使用此工号在内部邮件系统中发邮件联系公司员工，确认付款和确认信息。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>注意</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>如果是需要直接联系其他的外网邮箱，不是联系公司员工确认付款和确认信息，请填外网邮箱。必填项目</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收货地址，将提交给巧虎公司；必填项目，一般限制为公司地址。
-特殊情况可选其他地址;请点击选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订购类型 ，不同类型区别在于发的订购礼物不同。巧虎公司根据电话号码和小朋友信息管理订购。新用户请选新订。续订是指到期后接着订购。复活是指中断后恢复订购。对复活和续订要填对原来订购的手机号便于接着之前订购情况发后继版本，巧虎公司会按手机号查询到历史订单确认最终订购类型。将提交给巧虎公司。请点击选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订购周期，将提交给巧虎公司。新用户建议选1年（不可退订）。请点击选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小朋友性别 ， 将提交给巧虎公司；请点击选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订购产品的家长性别，将提交给巧虎公司；请点击选择</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -301,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -320,20 +355,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF4B4B4B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4B4B4B"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -341,8 +363,15 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -350,7 +379,21 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -358,11 +401,25 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4B4B4B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4B4B4B"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -408,22 +465,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,114 +906,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="63.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.75" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="79.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="48">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="57" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="str">
+        <f>IF(LEN(B1) =0,"必须选择或填写","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="str">
+        <f>IF(LEN(B2) =0,"必须选择或填写","")</f>
+        <v>必须选择或填写</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="str">
+        <f t="shared" ref="C2:C11" si="0">IF(LEN(B3) =0,"必须选择或填写","")</f>
+        <v>必须选择或填写</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>必须选择或填写</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90.75" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>必须选择或填写</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>必须选择或填写</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="str">
+        <f>IF(LEN(B10) &lt;&gt;11,"号码长度不对","")</f>
+        <v>号码长度不对</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="31.5" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="102" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="185.25">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" ht="48">
-      <c r="A3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="24">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="50.25" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" ht="24">
-      <c r="A11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="39" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" ht="84.75" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" ht="96">
-      <c r="A14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -987,123 +1094,124 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="44.25" customWidth="1"/>
+    <col min="1" max="1" width="72.125" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15">
+      <c r="A2" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" ht="15">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" ht="15">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" ht="15">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" ht="15">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="28.5">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:1" ht="15">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" ht="15">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:1" ht="15">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" ht="15">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:1" ht="15">
+      <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" ht="15">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" ht="15">
+      <c r="A14" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15">
+      <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15">
-      <c r="A14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="28.5">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:1" ht="15">
+      <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="28.5">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" ht="15">
+      <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:1" ht="15">
+      <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" ht="15">
+      <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:1" ht="15">
+      <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="28.5">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:1" ht="15">
+      <c r="A21" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:1" ht="15">
+      <c r="A22" s="9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
order add a column
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -15,17 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>1年期</t>
   </si>
   <si>
-    <t>小朋友姓名（可用昵称\小名，为了对应不同孩子的信息） ，将提交给巧虎公司</t>
-  </si>
-  <si>
-    <t>订购产品的家长姓名，代他人订请填实际订购人名字。将提交给巧虎公司；续订请填之前的家长名字如需修改请最后备注</t>
-  </si>
-  <si>
     <t>女</t>
   </si>
   <si>
@@ -104,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>订购类型 ，不同类型区别在于发的订购礼物不同。巧虎公司根据电话号码和小朋友信息管理订购。新用户请选新订。续订是指到期后接着订购。复活是指中断后恢复订购。对复活和续订要填对原来订购的手机号便于接着之前订购情况发后继版本，巧虎公司会按手机号查询到历史订单确认最终订购类型。将提交给巧虎公司。请点击选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>订购周期，将提交给巧虎公司。新用户建议选1年（不可退订）。请点击选择</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,11 +111,6 @@
   </si>
   <si>
     <t>手机号码 ，用于在巧虎公司订单系统查询之前的订单，确认本次订购方式，快递联系收货和用于对应售后服务，将提交给巧虎公司；复活或者续订用户如果这次要更换新的电话号码订购，请最后一项备注之前订购的电话号码。团购限制，一个手机号限订一份，除非同一个家庭的多个孩子可一个手机号码订多份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收货地址，将提交给巧虎公司；必填项目，一般限制为公司地址。
-特殊情况可选其他地址;请点击选择</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -164,25 +149,107 @@
   <si>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color rgb="FF4B4B4B"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>南京市雨花台区花神大道</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4B4B4B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4B4B4B"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新订</t>
+  </si>
+  <si>
+    <r>
+      <t>感谢您的填写，注意1-11项是</t>
+    </r>
+    <r>
+      <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
-      <t>联系邮箱</t>
+      <t>必填</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
+      <t>的。最后请确认上面填写的信息，特别是订购电话和小朋友生日，送货地址等重要信息无误后，使用常用邮箱发送到 qiaohu2013@qq.com  
+   确定价格后，您上面填的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>第3项的联系邮箱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>将收到确认收到团购信息和通知付款金额账号邮件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">。付款确认将统一在团购结束前发送。如果没收到上述邮件，请确认订购信息邮件是否发送成功，或联系邮箱 qiaohu2013@qq.com。
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同类型区别在于发的订购礼物不同。巧虎公司根据电话号码和小朋友信息管理订购。新用户请选新订。续订是指到期后接着订购。复活是指中断后恢复订购。对复活和续订要填对原来订购的手机号便于接着之前订购情况发后继版本，巧虎公司会按手机号查询到历史订单确认最终订购类型。将提交给巧虎公司。请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">。公司员工可填工号，如10088888，我将使用此工号在内部邮件系统中发邮件联系公司员工，确认付款和确认信息。
 </t>
     </r>
@@ -212,101 +279,68 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF4B4B4B"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>南京市雨花台区花神大道</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF4B4B4B"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF4B4B4B"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>号</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新订</t>
-  </si>
-  <si>
-    <r>
-      <t>感谢您的填写，注意1-11项是</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>必填</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>的。最后请确认上面填写的信息，特别是订购电话和小朋友生日，送货地址等重要信息无误后，使用常用邮箱发送到 qiaohu2013@qq.com  
-   确定价格后，您上面填的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>第3项的联系邮箱</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>将收到确认收到团购信息和通知付款金额账号邮件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">。付款确认将统一在团购结束前发送。如果没收到上述邮件，请确认订购信息邮件是否发送成功，或联系邮箱 qiaohu2013@qq.com。
-</t>
-    </r>
+    <t>小朋友姓名（可用昵称\小名，为了对应不同孩子的信息） ，将提交给巧虎公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购产品的家长姓名，代他人订请填实际订购人名字。将提交给巧虎公司；续订请填之前的家长名字如需修改请最后备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购产品的家长姓名，收件人名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收货地址，将提交给巧虎公司；必填项目，一般限制为公司地址。
+特殊情况可下拉到最后选择其他地址;请点击选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">订购类型 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司员工的名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小朋友姓名或者小名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小朋友性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小朋友生日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>家长性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订购电话，做收货和售后查询客户信息用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收货地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -314,7 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -399,8 +433,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +451,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,10 +490,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -454,17 +500,29 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,162 +946,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="86" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.8984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.69921875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="74.59765625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="68.400000000000006" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="2" t="str">
+    <row r="1" spans="1:4" ht="63.6" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="10" t="str">
         <f>IF(LEN(B1) =0,"必须选择或填写","")</f>
         <v/>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2" t="str">
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6">
+      <c r="A2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="10" t="str">
         <f>IF(LEN(B2) =0,"必须选择或填写","")</f>
         <v>必须选择或填写</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="62.4">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2" t="str">
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="62.4">
+      <c r="A3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10" t="str">
         <f t="shared" ref="C3:C11" si="0">IF(LEN(B3) =0,"必须选择或填写","")</f>
         <v>必须选择或填写</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6">
-      <c r="A4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.6">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="2" t="str">
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6">
+      <c r="A5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="10" t="str">
         <f t="shared" si="0"/>
         <v>必须选择或填写</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.6">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="str">
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="90.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2" t="str">
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90.75" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>必须选择或填写</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="31.2">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2" t="str">
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.2">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>必须选择或填写</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.6">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="str">
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6">
+      <c r="A9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="60.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2" t="str">
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60.75" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="10" t="str">
         <f>IF(LEN(B10) &lt;&gt;11,"号码长度不对","")</f>
         <v>号码长度不对</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="31.5" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="str">
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.5" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45.75" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="126" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="151.80000000000001" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" ht="126" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" ht="151.80000000000001" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1082,118 +1181,118 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="72.09765625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="72.09765625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="4" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="4" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="4" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="4" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="4" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="4" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="4" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1207,27 +1306,27 @@
   <legacyDrawing r:id="rId2"/>
   <legacyDrawingHF r:id="rId3"/>
   <controls>
-    <control shapeId="2049" r:id="rId4" name="Control 1"/>
-    <control shapeId="2050" r:id="rId5" name="Control 2"/>
-    <control shapeId="2051" r:id="rId6" name="Control 3"/>
-    <control shapeId="2052" r:id="rId7" name="Control 4"/>
-    <control shapeId="2053" r:id="rId8" name="Control 5"/>
-    <control shapeId="2054" r:id="rId9" name="Control 6"/>
-    <control shapeId="2055" r:id="rId10" name="Control 7"/>
-    <control shapeId="2056" r:id="rId11" name="Control 8"/>
-    <control shapeId="2057" r:id="rId12" name="Control 9"/>
-    <control shapeId="2058" r:id="rId13" name="Control 10"/>
+    <control shapeId="2069" r:id="rId4" name="Control 21"/>
+    <control shapeId="2068" r:id="rId5" name="Control 20"/>
+    <control shapeId="2067" r:id="rId6" name="Control 19"/>
+    <control shapeId="2066" r:id="rId7" name="Control 18"/>
+    <control shapeId="2065" r:id="rId8" name="Control 17"/>
+    <control shapeId="2064" r:id="rId9" name="Control 16"/>
+    <control shapeId="2063" r:id="rId10" name="Control 15"/>
+    <control shapeId="2062" r:id="rId11" name="Control 14"/>
+    <control shapeId="2061" r:id="rId12" name="Control 13"/>
+    <control shapeId="2060" r:id="rId13" name="Control 12"/>
     <control shapeId="2059" r:id="rId14" name="Control 11"/>
-    <control shapeId="2060" r:id="rId15" name="Control 12"/>
-    <control shapeId="2061" r:id="rId16" name="Control 13"/>
-    <control shapeId="2062" r:id="rId17" name="Control 14"/>
-    <control shapeId="2063" r:id="rId18" name="Control 15"/>
-    <control shapeId="2064" r:id="rId19" name="Control 16"/>
-    <control shapeId="2065" r:id="rId20" name="Control 17"/>
-    <control shapeId="2066" r:id="rId21" name="Control 18"/>
-    <control shapeId="2067" r:id="rId22" name="Control 19"/>
-    <control shapeId="2068" r:id="rId23" name="Control 20"/>
-    <control shapeId="2069" r:id="rId24" name="Control 21"/>
+    <control shapeId="2058" r:id="rId15" name="Control 10"/>
+    <control shapeId="2057" r:id="rId16" name="Control 9"/>
+    <control shapeId="2056" r:id="rId17" name="Control 8"/>
+    <control shapeId="2055" r:id="rId18" name="Control 7"/>
+    <control shapeId="2054" r:id="rId19" name="Control 6"/>
+    <control shapeId="2053" r:id="rId20" name="Control 5"/>
+    <control shapeId="2052" r:id="rId21" name="Control 4"/>
+    <control shapeId="2051" r:id="rId22" name="Control 3"/>
+    <control shapeId="2050" r:id="rId23" name="Control 2"/>
+    <control shapeId="2049" r:id="rId24" name="Control 1"/>
   </controls>
 </worksheet>
 </file>
</xml_diff>